<commit_message>
added elements of tidy dataset to codebook
</commit_message>
<xml_diff>
--- a/Tidy file Codebook and File Layout.xlsx
+++ b/Tidy file Codebook and File Layout.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Text\Coursea\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bears Everywhere\Course-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4224" windowWidth="23040" windowHeight="9504" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="5280" windowWidth="23040" windowHeight="9504" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Codebook" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="272">
   <si>
     <t>Data Codebook of movement measures across activities of daily living (Walking (level, up or downstairs), sitting, standing, laying)</t>
   </si>
@@ -814,12 +814,6 @@
     <t>filename: tidy</t>
   </si>
   <si>
-    <t>format: R written in R version 3.1.2</t>
-  </si>
-  <si>
-    <t>R software to read this file is available at:http://cran.r-project.org/ and is free of charge. Please follow</t>
-  </si>
-  <si>
     <t xml:space="preserve">See run_Analysis.R program for ETL details.  </t>
   </si>
   <si>
@@ -832,19 +826,103 @@
     <t>Date created: 11/18/2014</t>
   </si>
   <si>
-    <t>contents: mean of the variable for each subject's activity (walking, walking upstairs, walking downstairs, sitting standing, laying)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">measured by samsumg II smartphone readings from acceleratometer and gyroscope. All values are numeric. </t>
-  </si>
-  <si>
     <t xml:space="preserve">SubjectID and ActivityID are integers while all other variables are numbers with a decimal point, e.g., -0.2853077700.  No missing values (NA). </t>
   </si>
   <si>
     <t>see codebook tab for descriptions of variable or column headings</t>
   </si>
   <si>
-    <t>Tidy dataset file layout</t>
+    <t>tidy.txt dataset file layout</t>
+  </si>
+  <si>
+    <t>format: text comma delimited, 264 kb</t>
+  </si>
+  <si>
+    <t>contents:  A summary (mean) of select activity measures across 128 observations from 30 subjects over 5 activities.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mean of the variable for each subject's activity (walking, .walking upstairs, walking downstairs, sitting standing, laying)</t>
+  </si>
+  <si>
+    <t>The summary observations (means of select activity variable) are derived from original raw data contained in</t>
+  </si>
+  <si>
+    <t>legacy (unzipped) folders UCI HAR Dataset\(test or train)\Inertial Signals</t>
+  </si>
+  <si>
+    <t>Study Design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Human Activity Recognition using smartphones database describes 30 subjects aged 19 - 48 performing </t>
+  </si>
+  <si>
+    <t>activities of daily living (adl), e.g., walking upstairs, walking downstairs, sitting, standing, laying.</t>
+  </si>
+  <si>
+    <t>Linear acceration data of these adls were collected by the embedded accelerometer on each subjects</t>
+  </si>
+  <si>
+    <t>samsumg galaxy SII smartphone. 3 axial angular velocity data of these ads were collected by the</t>
+  </si>
+  <si>
+    <t xml:space="preserve">embedded gyroscope of the samsung phone. </t>
+  </si>
+  <si>
+    <t>to refine and sharpen the signal, allowing gravitational and body motion components to be separated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These sensor signals (triaxial  and bodily acceleration and triaxial angular velocity) from the acceleratometer </t>
+  </si>
+  <si>
+    <t>and gyroscope were refined by apply noise filters</t>
+  </si>
+  <si>
+    <t>These signals were further calculated into various features (total of 561)  from their associated time and frequency domains.</t>
+  </si>
+  <si>
+    <t>citation/source information:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Davide Anguita, Alessandro Ghio, Luca Oneto, Xavier Parra and Jorge L. Reyes-Ortiz. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human Activity Recognition on Smartphones using a Multiclass Hardware-Friendly Support Vector Machine. </t>
+  </si>
+  <si>
+    <t>International Workshop of Ambient Assisted Living (IWAAL 2012). Vitoria-Gasteiz, Spain. Dec 2012</t>
+  </si>
+  <si>
+    <t>contact information:</t>
+  </si>
+  <si>
+    <t>Jorge L. Reyes-Ortiz, Davide Anguita, Alessandro Ghio, Luca Oneto.</t>
+  </si>
+  <si>
+    <t>Smartlab - Non Linear Complex Systems Laboratory</t>
+  </si>
+  <si>
+    <t>DITEN - Università degli Studi di Genova.</t>
+  </si>
+  <si>
+    <t>Via Opera Pia 11A, I-16145, Genoa, Italy.</t>
+  </si>
+  <si>
+    <t>activityrecognition@smartlab.ws</t>
+  </si>
+  <si>
+    <t>www.smartlab.ws</t>
+  </si>
+  <si>
+    <t>Accelerometer data are in standard gravity units. Body acceleration signals are calculated by subtracting gravity from total acceleratin</t>
+  </si>
+  <si>
+    <t>Angular velocity data (from the gyroscope) are in radians/second units.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measured by samsung II smartphone readings from acceleratometer and gyroscope. All values are numeric. </t>
+  </si>
+  <si>
+    <t>The dataset is ramdomly partitioned into training (70% of all subjects) and test(30% of all subjects) partitions.</t>
   </si>
 </sst>
 </file>
@@ -1010,8 +1088,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" textRotation="44"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1020,34 +1121,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" textRotation="44"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1382,35 +1460,35 @@
     </row>
     <row r="3" spans="2:13" s="1" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="2"/>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
     </row>
     <row r="4" spans="2:13" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="20"/>
+      <c r="F4" s="17"/>
       <c r="G4" s="4"/>
       <c r="H4" s="21" t="s">
         <v>3</v>
       </c>
       <c r="I4" s="21"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="20"/>
+      <c r="L4" s="17"/>
     </row>
     <row r="5" spans="2:13" s="1" customFormat="1" ht="38.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="6"/>
@@ -1458,19 +1536,19 @@
       <c r="M6" s="10"/>
     </row>
     <row r="7" spans="2:13" s="1" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
       <c r="M7" s="10"/>
     </row>
     <row r="8" spans="2:13" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
@@ -1666,13 +1744,13 @@
       <c r="D23" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
     </row>
     <row r="24" spans="2:11" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C24" t="s">
@@ -1681,13 +1759,13 @@
       <c r="D24" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
     </row>
     <row r="25" spans="2:11" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C25" t="s">
@@ -1696,13 +1774,13 @@
       <c r="D25" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
     </row>
     <row r="26" spans="2:11" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C26" t="s">
@@ -1711,13 +1789,13 @@
       <c r="D26" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
     </row>
     <row r="27" spans="2:11" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C27" t="s">
@@ -1726,13 +1804,13 @@
       <c r="D27" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
     </row>
     <row r="28" spans="2:11" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C28" t="s">
@@ -1741,13 +1819,13 @@
       <c r="D28" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
     </row>
     <row r="29" spans="2:11" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B29" s="3" t="s">
@@ -1864,35 +1942,35 @@
     </row>
     <row r="38" spans="2:13" s="1" customFormat="1" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B38" s="2"/>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="20"/>
     </row>
     <row r="39" spans="2:13" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="E39" s="20" t="s">
+      <c r="E39" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F39" s="20"/>
+      <c r="F39" s="17"/>
       <c r="G39" s="4"/>
       <c r="H39" s="21" t="s">
         <v>3</v>
       </c>
       <c r="I39" s="21"/>
       <c r="J39" s="5"/>
-      <c r="K39" s="20" t="s">
+      <c r="K39" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="L39" s="20"/>
+      <c r="L39" s="17"/>
     </row>
     <row r="40" spans="2:13" s="1" customFormat="1" ht="38.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B40" s="6"/>
@@ -1979,13 +2057,13 @@
       <c r="D45" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E45" s="14" t="s">
+      <c r="E45" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="20"/>
     </row>
     <row r="46" spans="2:13" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C46" t="s">
@@ -1994,13 +2072,13 @@
       <c r="D46" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E46" s="14" t="s">
+      <c r="E46" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="20"/>
     </row>
     <row r="47" spans="2:13" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C47" t="s">
@@ -2009,13 +2087,13 @@
       <c r="D47" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E47" s="14" t="s">
+      <c r="E47" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="20"/>
     </row>
     <row r="48" spans="2:13" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B48" s="18" t="s">
@@ -2049,35 +2127,35 @@
     </row>
     <row r="50" spans="2:13" s="1" customFormat="1" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B50" s="2"/>
-      <c r="C50" s="14" t="s">
+      <c r="C50" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14"/>
-      <c r="L50" s="14"/>
-      <c r="M50" s="14"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="20"/>
+      <c r="L50" s="20"/>
+      <c r="M50" s="20"/>
     </row>
     <row r="51" spans="2:13" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="E51" s="20" t="s">
+      <c r="E51" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F51" s="20"/>
+      <c r="F51" s="17"/>
       <c r="G51" s="4"/>
       <c r="H51" s="21" t="s">
         <v>3</v>
       </c>
       <c r="I51" s="21"/>
       <c r="J51" s="5"/>
-      <c r="K51" s="20" t="s">
+      <c r="K51" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="L51" s="20"/>
+      <c r="L51" s="17"/>
     </row>
     <row r="52" spans="2:13" s="1" customFormat="1" ht="38.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B52" s="6"/>
@@ -2139,13 +2217,13 @@
       <c r="D55" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E55" s="14" t="s">
+      <c r="E55" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="20"/>
+      <c r="I55" s="20"/>
     </row>
     <row r="56" spans="2:13" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B56" s="3" t="s">
@@ -2213,13 +2291,13 @@
       <c r="D60" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E60" s="14" t="s">
+      <c r="E60" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="14"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="20"/>
+      <c r="I60" s="20"/>
     </row>
     <row r="61" spans="2:13" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C61" t="s">
@@ -2228,13 +2306,13 @@
       <c r="D61" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E61" s="14" t="s">
+      <c r="E61" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="F61" s="14"/>
-      <c r="G61" s="14"/>
-      <c r="H61" s="14"/>
-      <c r="I61" s="14"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="20"/>
+      <c r="H61" s="20"/>
+      <c r="I61" s="20"/>
     </row>
     <row r="62" spans="2:13" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B62" s="3" t="s">
@@ -2340,35 +2418,35 @@
     </row>
     <row r="70" spans="2:13" s="1" customFormat="1" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B70" s="2"/>
-      <c r="C70" s="14" t="s">
+      <c r="C70" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="D70" s="14"/>
-      <c r="E70" s="14"/>
-      <c r="F70" s="14"/>
-      <c r="G70" s="14"/>
-      <c r="H70" s="14"/>
-      <c r="I70" s="14"/>
-      <c r="J70" s="14"/>
-      <c r="K70" s="14"/>
-      <c r="L70" s="14"/>
-      <c r="M70" s="14"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="20"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="20"/>
+      <c r="H70" s="20"/>
+      <c r="I70" s="20"/>
+      <c r="J70" s="20"/>
+      <c r="K70" s="20"/>
+      <c r="L70" s="20"/>
+      <c r="M70" s="20"/>
     </row>
     <row r="71" spans="2:13" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="E71" s="20" t="s">
+      <c r="E71" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F71" s="20"/>
+      <c r="F71" s="17"/>
       <c r="G71" s="4"/>
       <c r="H71" s="21" t="s">
         <v>3</v>
       </c>
       <c r="I71" s="21"/>
       <c r="J71" s="5"/>
-      <c r="K71" s="20" t="s">
+      <c r="K71" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="L71" s="20"/>
+      <c r="L71" s="17"/>
     </row>
     <row r="72" spans="2:13" s="1" customFormat="1" ht="38.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B72" s="6"/>
@@ -2452,13 +2530,13 @@
       <c r="D77" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E77" s="14" t="s">
+      <c r="E77" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="F77" s="14"/>
-      <c r="G77" s="14"/>
-      <c r="H77" s="14"/>
-      <c r="I77" s="14"/>
+      <c r="F77" s="20"/>
+      <c r="G77" s="20"/>
+      <c r="H77" s="20"/>
+      <c r="I77" s="20"/>
     </row>
     <row r="78" spans="2:13" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C78" t="s">
@@ -2467,13 +2545,13 @@
       <c r="D78" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E78" s="14" t="s">
+      <c r="E78" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="F78" s="14"/>
-      <c r="G78" s="14"/>
-      <c r="H78" s="14"/>
-      <c r="I78" s="14"/>
+      <c r="F78" s="20"/>
+      <c r="G78" s="20"/>
+      <c r="H78" s="20"/>
+      <c r="I78" s="20"/>
       <c r="J78" s="13"/>
     </row>
     <row r="79" spans="2:13" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
@@ -2483,13 +2561,13 @@
       <c r="D79" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E79" s="14" t="s">
+      <c r="E79" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="F79" s="14"/>
-      <c r="G79" s="14"/>
-      <c r="H79" s="14"/>
-      <c r="I79" s="14"/>
+      <c r="F79" s="20"/>
+      <c r="G79" s="20"/>
+      <c r="H79" s="20"/>
+      <c r="I79" s="20"/>
       <c r="J79" s="13"/>
     </row>
     <row r="80" spans="2:13" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
@@ -2516,13 +2594,13 @@
       <c r="D81" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E81" s="14" t="s">
+      <c r="E81" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="F81" s="14"/>
-      <c r="G81" s="14"/>
-      <c r="H81" s="14"/>
-      <c r="I81" s="14"/>
+      <c r="F81" s="20"/>
+      <c r="G81" s="20"/>
+      <c r="H81" s="20"/>
+      <c r="I81" s="20"/>
     </row>
     <row r="82" spans="2:13" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C82" t="s">
@@ -2531,13 +2609,13 @@
       <c r="D82" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E82" s="14" t="s">
+      <c r="E82" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="F82" s="14"/>
-      <c r="G82" s="14"/>
-      <c r="H82" s="14"/>
-      <c r="I82" s="14"/>
+      <c r="F82" s="20"/>
+      <c r="G82" s="20"/>
+      <c r="H82" s="20"/>
+      <c r="I82" s="20"/>
     </row>
     <row r="83" spans="2:13" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C83" t="s">
@@ -2546,13 +2624,13 @@
       <c r="D83" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E83" s="14" t="s">
+      <c r="E83" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="F83" s="14"/>
-      <c r="G83" s="14"/>
-      <c r="H83" s="14"/>
-      <c r="I83" s="14"/>
+      <c r="F83" s="20"/>
+      <c r="G83" s="20"/>
+      <c r="H83" s="20"/>
+      <c r="I83" s="20"/>
     </row>
     <row r="84" spans="2:13" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C84" t="s">
@@ -2561,13 +2639,13 @@
       <c r="D84" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E84" s="14" t="s">
+      <c r="E84" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="F84" s="14"/>
-      <c r="G84" s="14"/>
-      <c r="H84" s="14"/>
-      <c r="I84" s="14"/>
+      <c r="F84" s="20"/>
+      <c r="G84" s="20"/>
+      <c r="H84" s="20"/>
+      <c r="I84" s="20"/>
     </row>
     <row r="85" spans="2:13" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C85" t="s">
@@ -2576,13 +2654,13 @@
       <c r="D85" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E85" s="14" t="s">
+      <c r="E85" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="F85" s="14"/>
-      <c r="G85" s="14"/>
-      <c r="H85" s="14"/>
-      <c r="I85" s="14"/>
+      <c r="F85" s="20"/>
+      <c r="G85" s="20"/>
+      <c r="H85" s="20"/>
+      <c r="I85" s="20"/>
     </row>
     <row r="86" spans="2:13" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C86" t="s">
@@ -2591,13 +2669,13 @@
       <c r="D86" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E86" s="14" t="s">
+      <c r="E86" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="F86" s="14"/>
-      <c r="G86" s="14"/>
-      <c r="H86" s="14"/>
-      <c r="I86" s="14"/>
+      <c r="F86" s="20"/>
+      <c r="G86" s="20"/>
+      <c r="H86" s="20"/>
+      <c r="I86" s="20"/>
     </row>
     <row r="87" spans="2:13" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B87" s="18" t="s">
@@ -2631,35 +2709,35 @@
     </row>
     <row r="89" spans="2:13" s="1" customFormat="1" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B89" s="2"/>
-      <c r="C89" s="14" t="s">
+      <c r="C89" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="D89" s="14"/>
-      <c r="E89" s="14"/>
-      <c r="F89" s="14"/>
-      <c r="G89" s="14"/>
-      <c r="H89" s="14"/>
-      <c r="I89" s="14"/>
-      <c r="J89" s="14"/>
-      <c r="K89" s="14"/>
-      <c r="L89" s="14"/>
-      <c r="M89" s="14"/>
+      <c r="D89" s="20"/>
+      <c r="E89" s="20"/>
+      <c r="F89" s="20"/>
+      <c r="G89" s="20"/>
+      <c r="H89" s="20"/>
+      <c r="I89" s="20"/>
+      <c r="J89" s="20"/>
+      <c r="K89" s="20"/>
+      <c r="L89" s="20"/>
+      <c r="M89" s="20"/>
     </row>
     <row r="90" spans="2:13" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="E90" s="20" t="s">
+      <c r="E90" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F90" s="20"/>
+      <c r="F90" s="17"/>
       <c r="G90" s="4"/>
       <c r="H90" s="21" t="s">
         <v>3</v>
       </c>
       <c r="I90" s="21"/>
       <c r="J90" s="5"/>
-      <c r="K90" s="20" t="s">
+      <c r="K90" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="L90" s="20"/>
+      <c r="L90" s="17"/>
     </row>
     <row r="91" spans="2:13" s="1" customFormat="1" ht="38.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B91" s="6"/>
@@ -2835,13 +2913,13 @@
       <c r="D103" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E103" s="14" t="s">
+      <c r="E103" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="F103" s="14"/>
-      <c r="G103" s="14"/>
-      <c r="H103" s="14"/>
-      <c r="I103" s="14"/>
+      <c r="F103" s="20"/>
+      <c r="G103" s="20"/>
+      <c r="H103" s="20"/>
+      <c r="I103" s="20"/>
     </row>
     <row r="104" spans="2:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C104" t="s">
@@ -2850,13 +2928,13 @@
       <c r="D104" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E104" s="14" t="s">
+      <c r="E104" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="F104" s="14"/>
-      <c r="G104" s="14"/>
-      <c r="H104" s="14"/>
-      <c r="I104" s="14"/>
+      <c r="F104" s="20"/>
+      <c r="G104" s="20"/>
+      <c r="H104" s="20"/>
+      <c r="I104" s="20"/>
     </row>
     <row r="105" spans="2:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B105" s="3" t="s">
@@ -2913,13 +2991,13 @@
       <c r="D108" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E108" s="14" t="s">
+      <c r="E108" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="F108" s="14"/>
-      <c r="G108" s="14"/>
-      <c r="H108" s="14"/>
-      <c r="I108" s="14"/>
+      <c r="F108" s="20"/>
+      <c r="G108" s="20"/>
+      <c r="H108" s="20"/>
+      <c r="I108" s="20"/>
     </row>
     <row r="109" spans="2:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C109" t="s">
@@ -2928,212 +3006,164 @@
       <c r="D109" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E109" s="14" t="s">
+      <c r="E109" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="F109" s="14"/>
-      <c r="G109" s="14"/>
-      <c r="H109" s="14"/>
-      <c r="I109" s="14"/>
+      <c r="F109" s="20"/>
+      <c r="G109" s="20"/>
+      <c r="H109" s="20"/>
+      <c r="I109" s="20"/>
     </row>
     <row r="110" spans="2:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C110" t="s">
         <v>200</v>
       </c>
-      <c r="E110" s="15" t="s">
+      <c r="E110" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="F110" s="16"/>
-      <c r="G110" s="16"/>
-      <c r="H110" s="16"/>
-      <c r="I110" s="16"/>
+      <c r="F110" s="25"/>
+      <c r="G110" s="25"/>
+      <c r="H110" s="25"/>
+      <c r="I110" s="25"/>
     </row>
     <row r="111" spans="2:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C111" t="s">
         <v>201</v>
       </c>
-      <c r="E111" s="16"/>
-      <c r="F111" s="16"/>
-      <c r="G111" s="16"/>
-      <c r="H111" s="16"/>
-      <c r="I111" s="16"/>
+      <c r="E111" s="25"/>
+      <c r="F111" s="25"/>
+      <c r="G111" s="25"/>
+      <c r="H111" s="25"/>
+      <c r="I111" s="25"/>
     </row>
     <row r="112" spans="2:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C112" t="s">
         <v>202</v>
       </c>
-      <c r="E112" s="16"/>
-      <c r="F112" s="16"/>
-      <c r="G112" s="16"/>
-      <c r="H112" s="16"/>
-      <c r="I112" s="16"/>
+      <c r="E112" s="25"/>
+      <c r="F112" s="25"/>
+      <c r="G112" s="25"/>
+      <c r="H112" s="25"/>
+      <c r="I112" s="25"/>
     </row>
     <row r="113" spans="2:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C113" t="s">
         <v>203</v>
       </c>
-      <c r="E113" s="16"/>
-      <c r="F113" s="16"/>
-      <c r="G113" s="16"/>
-      <c r="H113" s="16"/>
-      <c r="I113" s="16"/>
+      <c r="E113" s="25"/>
+      <c r="F113" s="25"/>
+      <c r="G113" s="25"/>
+      <c r="H113" s="25"/>
+      <c r="I113" s="25"/>
     </row>
     <row r="114" spans="2:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C114" t="s">
         <v>204</v>
       </c>
-      <c r="E114" s="16"/>
-      <c r="F114" s="16"/>
-      <c r="G114" s="16"/>
-      <c r="H114" s="16"/>
-      <c r="I114" s="16"/>
+      <c r="E114" s="25"/>
+      <c r="F114" s="25"/>
+      <c r="G114" s="25"/>
+      <c r="H114" s="25"/>
+      <c r="I114" s="25"/>
     </row>
     <row r="115" spans="2:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C115" t="s">
         <v>205</v>
       </c>
-      <c r="E115" s="16"/>
-      <c r="F115" s="16"/>
-      <c r="G115" s="16"/>
-      <c r="H115" s="16"/>
-      <c r="I115" s="16"/>
+      <c r="E115" s="25"/>
+      <c r="F115" s="25"/>
+      <c r="G115" s="25"/>
+      <c r="H115" s="25"/>
+      <c r="I115" s="25"/>
     </row>
     <row r="116" spans="2:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C116" t="s">
         <v>206</v>
       </c>
-      <c r="E116" s="16"/>
-      <c r="F116" s="16"/>
-      <c r="G116" s="16"/>
-      <c r="H116" s="16"/>
-      <c r="I116" s="16"/>
+      <c r="E116" s="25"/>
+      <c r="F116" s="25"/>
+      <c r="G116" s="25"/>
+      <c r="H116" s="25"/>
+      <c r="I116" s="25"/>
     </row>
     <row r="117" spans="2:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B117" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E117" s="17" t="s">
+      <c r="E117" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="F117" s="17"/>
-      <c r="G117" s="17"/>
-      <c r="H117" s="17"/>
-      <c r="I117" s="17"/>
-      <c r="J117" s="17"/>
-      <c r="K117" s="17"/>
-      <c r="L117" s="17"/>
+      <c r="F117" s="23"/>
+      <c r="G117" s="23"/>
+      <c r="H117" s="23"/>
+      <c r="I117" s="23"/>
+      <c r="J117" s="23"/>
+      <c r="K117" s="23"/>
+      <c r="L117" s="23"/>
     </row>
     <row r="118" spans="2:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B118" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E118" s="14" t="s">
+      <c r="E118" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F118" s="14"/>
-      <c r="G118" s="14"/>
-      <c r="H118" s="14"/>
-      <c r="I118" s="14"/>
-      <c r="J118" s="14"/>
-      <c r="K118" s="14"/>
-      <c r="L118" s="14"/>
+      <c r="F118" s="20"/>
+      <c r="G118" s="20"/>
+      <c r="H118" s="20"/>
+      <c r="I118" s="20"/>
+      <c r="J118" s="20"/>
+      <c r="K118" s="20"/>
+      <c r="L118" s="20"/>
     </row>
     <row r="119" spans="2:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B119" s="14" t="s">
+      <c r="B119" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C119" s="14"/>
-      <c r="D119" s="14"/>
-      <c r="E119" s="14"/>
-      <c r="F119" s="14"/>
-      <c r="G119" s="14"/>
-      <c r="H119" s="14"/>
-      <c r="I119" s="14"/>
-      <c r="J119" s="14"/>
-      <c r="K119" s="14"/>
-      <c r="L119" s="14"/>
+      <c r="C119" s="20"/>
+      <c r="D119" s="20"/>
+      <c r="E119" s="20"/>
+      <c r="F119" s="20"/>
+      <c r="G119" s="20"/>
+      <c r="H119" s="20"/>
+      <c r="I119" s="20"/>
+      <c r="J119" s="20"/>
+      <c r="K119" s="20"/>
+      <c r="L119" s="20"/>
     </row>
     <row r="120" spans="2:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B120" s="14" t="s">
+      <c r="B120" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C120" s="14"/>
-      <c r="D120" s="14"/>
-      <c r="E120" s="14"/>
-      <c r="F120" s="14"/>
-      <c r="G120" s="14"/>
-      <c r="H120" s="14"/>
-      <c r="I120" s="14"/>
-      <c r="J120" s="14"/>
-      <c r="K120" s="14"/>
-      <c r="L120" s="14"/>
+      <c r="C120" s="20"/>
+      <c r="D120" s="20"/>
+      <c r="E120" s="20"/>
+      <c r="F120" s="20"/>
+      <c r="G120" s="20"/>
+      <c r="H120" s="20"/>
+      <c r="I120" s="20"/>
+      <c r="J120" s="20"/>
+      <c r="K120" s="20"/>
+      <c r="L120" s="20"/>
     </row>
     <row r="121" spans="2:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B121" s="14" t="s">
+      <c r="B121" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C121" s="14"/>
-      <c r="D121" s="14"/>
-      <c r="E121" s="14"/>
-      <c r="F121" s="14"/>
-      <c r="G121" s="14"/>
-      <c r="H121" s="14"/>
-      <c r="I121" s="14"/>
-      <c r="J121" s="14"/>
-      <c r="K121" s="14"/>
-      <c r="L121" s="14"/>
+      <c r="C121" s="20"/>
+      <c r="D121" s="20"/>
+      <c r="E121" s="20"/>
+      <c r="F121" s="20"/>
+      <c r="G121" s="20"/>
+      <c r="H121" s="20"/>
+      <c r="I121" s="20"/>
+      <c r="J121" s="20"/>
+      <c r="K121" s="20"/>
+      <c r="L121" s="20"/>
     </row>
     <row r="122" spans="2:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="B1:L1"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="C3:M3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="B6:L6"/>
-    <mergeCell ref="B7:L7"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="C38:M38"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="B68:L68"/>
-    <mergeCell ref="B69:L69"/>
-    <mergeCell ref="C70:M70"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="H71:I71"/>
-    <mergeCell ref="K71:L71"/>
-    <mergeCell ref="E117:L117"/>
-    <mergeCell ref="E118:L118"/>
-    <mergeCell ref="B119:L119"/>
-    <mergeCell ref="B120:L120"/>
-    <mergeCell ref="B121:L121"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E45:I45"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="E46:I46"/>
-    <mergeCell ref="E47:I47"/>
-    <mergeCell ref="E55:I55"/>
-    <mergeCell ref="E60:I60"/>
-    <mergeCell ref="E61:I61"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
-    <mergeCell ref="C50:M50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="K51:L51"/>
-    <mergeCell ref="E78:I78"/>
-    <mergeCell ref="E79:I79"/>
-    <mergeCell ref="E77:I77"/>
-    <mergeCell ref="E81:I81"/>
-    <mergeCell ref="E82:I82"/>
     <mergeCell ref="E104:I104"/>
     <mergeCell ref="E108:I108"/>
     <mergeCell ref="E109:I109"/>
@@ -3149,6 +3179,54 @@
     <mergeCell ref="E90:F90"/>
     <mergeCell ref="H90:I90"/>
     <mergeCell ref="K90:L90"/>
+    <mergeCell ref="E78:I78"/>
+    <mergeCell ref="E79:I79"/>
+    <mergeCell ref="E77:I77"/>
+    <mergeCell ref="E81:I81"/>
+    <mergeCell ref="E82:I82"/>
+    <mergeCell ref="E46:I46"/>
+    <mergeCell ref="E47:I47"/>
+    <mergeCell ref="E55:I55"/>
+    <mergeCell ref="E60:I60"/>
+    <mergeCell ref="E61:I61"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="C50:M50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="K51:L51"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E45:I45"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="E117:L117"/>
+    <mergeCell ref="E118:L118"/>
+    <mergeCell ref="B119:L119"/>
+    <mergeCell ref="B120:L120"/>
+    <mergeCell ref="B121:L121"/>
+    <mergeCell ref="B68:L68"/>
+    <mergeCell ref="B69:L69"/>
+    <mergeCell ref="C70:M70"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="H71:I71"/>
+    <mergeCell ref="K71:L71"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="C3:M3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="B6:L6"/>
+    <mergeCell ref="B7:L7"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="C38:M38"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3160,10 +3238,10 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="D2:CO15"/>
+  <dimension ref="D2:CO42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.1640625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -3173,15 +3251,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:93" ht="91.8" x14ac:dyDescent="1.65">
-      <c r="G2" s="27" t="s">
-        <v>245</v>
+      <c r="G2" s="16" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="4:93" x14ac:dyDescent="0.35">
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="26" t="s">
         <v>216</v>
       </c>
-      <c r="E3" s="23"/>
+      <c r="E3" s="26"/>
       <c r="F3">
         <v>1</v>
       </c>
@@ -3447,273 +3525,273 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="4:93" s="25" customFormat="1" ht="169.2" x14ac:dyDescent="0.35">
-      <c r="D4" s="24" t="s">
+    <row r="4" spans="4:93" s="14" customFormat="1" ht="169.2" x14ac:dyDescent="0.35">
+      <c r="D4" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25" t="s">
+      <c r="E4" s="27"/>
+      <c r="F4" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="K4" s="25" t="s">
+      <c r="K4" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="M4" s="25" t="s">
+      <c r="M4" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="O4" s="25" t="s">
+      <c r="O4" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="Q4" s="25" t="s">
+      <c r="Q4" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="R4" s="25" t="s">
+      <c r="R4" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="S4" s="25" t="s">
+      <c r="S4" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="U4" s="25" t="s">
+      <c r="U4" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="V4" s="25" t="s">
+      <c r="V4" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="W4" s="25" t="s">
+      <c r="W4" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="X4" s="25" t="s">
+      <c r="X4" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="Y4" s="25" t="s">
+      <c r="Y4" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="Z4" s="25" t="s">
+      <c r="Z4" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="AA4" s="25" t="s">
+      <c r="AA4" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="AB4" s="25" t="s">
+      <c r="AB4" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="AC4" s="25" t="s">
+      <c r="AC4" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="AD4" s="25" t="s">
+      <c r="AD4" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="AE4" s="25" t="s">
+      <c r="AE4" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="AF4" s="25" t="s">
+      <c r="AF4" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="AG4" s="25" t="s">
+      <c r="AG4" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="AH4" s="25" t="s">
+      <c r="AH4" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="AI4" s="25" t="s">
+      <c r="AI4" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="AJ4" s="25" t="s">
+      <c r="AJ4" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="AK4" s="25" t="s">
+      <c r="AK4" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="AL4" s="25" t="s">
+      <c r="AL4" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="AM4" s="25" t="s">
+      <c r="AM4" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="AN4" s="25" t="s">
+      <c r="AN4" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="AO4" s="25" t="s">
+      <c r="AO4" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="AP4" s="25" t="s">
+      <c r="AP4" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="AQ4" s="25" t="s">
+      <c r="AQ4" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="AR4" s="25" t="s">
+      <c r="AR4" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="AS4" s="25" t="s">
+      <c r="AS4" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="AT4" s="25" t="s">
+      <c r="AT4" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="AU4" s="25" t="s">
+      <c r="AU4" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="AV4" s="25" t="s">
+      <c r="AV4" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="AW4" s="25" t="s">
+      <c r="AW4" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="AX4" s="25" t="s">
+      <c r="AX4" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="AY4" s="25" t="s">
+      <c r="AY4" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="AZ4" s="25" t="s">
+      <c r="AZ4" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="BA4" s="25" t="s">
+      <c r="BA4" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="BB4" s="25" t="s">
+      <c r="BB4" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="BC4" s="25" t="s">
+      <c r="BC4" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="BD4" s="25" t="s">
+      <c r="BD4" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="BE4" s="25" t="s">
+      <c r="BE4" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="BF4" s="25" t="s">
+      <c r="BF4" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="BG4" s="25" t="s">
+      <c r="BG4" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="BH4" s="25" t="s">
+      <c r="BH4" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="BI4" s="25" t="s">
+      <c r="BI4" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="BJ4" s="25" t="s">
+      <c r="BJ4" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="BK4" s="25" t="s">
+      <c r="BK4" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="BL4" s="25" t="s">
+      <c r="BL4" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="BM4" s="25" t="s">
+      <c r="BM4" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="BN4" s="25" t="s">
+      <c r="BN4" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="BO4" s="25" t="s">
+      <c r="BO4" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="BP4" s="25" t="s">
+      <c r="BP4" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="BQ4" s="25" t="s">
+      <c r="BQ4" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="BR4" s="25" t="s">
+      <c r="BR4" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="BS4" s="25" t="s">
+      <c r="BS4" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="BT4" s="25" t="s">
+      <c r="BT4" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="BU4" s="25" t="s">
+      <c r="BU4" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="BV4" s="25" t="s">
+      <c r="BV4" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="BW4" s="25" t="s">
+      <c r="BW4" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="BX4" s="25" t="s">
+      <c r="BX4" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="BY4" s="25" t="s">
+      <c r="BY4" s="14" t="s">
         <v>229</v>
       </c>
-      <c r="BZ4" s="25" t="s">
+      <c r="BZ4" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="CA4" s="25" t="s">
+      <c r="CA4" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="CB4" s="25" t="s">
+      <c r="CB4" s="14" t="s">
         <v>230</v>
       </c>
-      <c r="CC4" s="25" t="s">
+      <c r="CC4" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="CD4" s="25" t="s">
+      <c r="CD4" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="CE4" s="25" t="s">
+      <c r="CE4" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="CF4" s="25" t="s">
+      <c r="CF4" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="CG4" s="25" t="s">
+      <c r="CG4" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="CH4" s="25" t="s">
+      <c r="CH4" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="CI4" s="25" t="s">
+      <c r="CI4" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="CJ4" s="25" t="s">
+      <c r="CJ4" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="CK4" s="25" t="s">
+      <c r="CK4" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="CL4" s="25" t="s">
+      <c r="CL4" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="CM4" s="25" t="s">
+      <c r="CM4" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="CN4" s="25" t="s">
+      <c r="CN4" s="14" t="s">
         <v>205</v>
       </c>
-      <c r="CO4" s="25" t="s">
+      <c r="CO4" s="14" t="s">
         <v>206</v>
       </c>
     </row>
@@ -3724,55 +3802,198 @@
     </row>
     <row r="6" spans="4:93" x14ac:dyDescent="0.35">
       <c r="F6" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="4:93" x14ac:dyDescent="0.35">
       <c r="F7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="4:93" x14ac:dyDescent="0.35">
       <c r="F8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="4:93" x14ac:dyDescent="0.35">
       <c r="F9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="4:93" x14ac:dyDescent="0.35">
+      <c r="F10" s="15" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="10" spans="4:93" x14ac:dyDescent="0.35">
-      <c r="F10" t="s">
+    <row r="11" spans="4:93" x14ac:dyDescent="0.35">
+      <c r="F11" s="15" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="12" spans="4:93" x14ac:dyDescent="0.35">
+      <c r="F12" s="15"/>
+      <c r="G12" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="13" spans="4:93" x14ac:dyDescent="0.35">
+      <c r="F13" s="15"/>
+      <c r="G13" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="14" spans="4:93" x14ac:dyDescent="0.35">
+      <c r="F14" s="15"/>
+      <c r="G14" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="4:93" x14ac:dyDescent="0.35">
+      <c r="F15" s="15"/>
+      <c r="G15" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="16" spans="4:93" x14ac:dyDescent="0.35">
+      <c r="F16" s="15"/>
+      <c r="G16" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="F17" s="15"/>
+      <c r="G17" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="F18" s="15"/>
+      <c r="G18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="F19" s="15"/>
+      <c r="G19" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="F20" s="15"/>
+      <c r="G20" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="F21" s="15"/>
+      <c r="G21" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="F22" s="15"/>
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="G24" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="G25" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="G26" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="G27" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="G28" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="G29" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="30" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="G30" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="11" spans="4:93" x14ac:dyDescent="0.35">
-      <c r="F11" s="26" t="s">
+    <row r="31" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="G31" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="12" spans="4:93" x14ac:dyDescent="0.35">
-      <c r="E12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="13" spans="4:93" x14ac:dyDescent="0.35">
-      <c r="G13" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="14" spans="4:93" x14ac:dyDescent="0.35">
-      <c r="G14" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="15" spans="4:93" x14ac:dyDescent="0.35">
-      <c r="G15" t="s">
-        <v>244</v>
+    <row r="32" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="F32" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="33" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="G33" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="34" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="G34" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="35" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="G35" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="36" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="F36" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="37" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="H37" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="38" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="H38" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="39" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="H39" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="40" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="H40" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="41" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="H41" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="42" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="H42" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>